<commit_message>
enemy and boss things
</commit_message>
<xml_diff>
--- a/PsychShift/Assets/Editor/CSV/EnemyExcelChart.xlsx
+++ b/PsychShift/Assets/Editor/CSV/EnemyExcelChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxth\OneDrive\Desktop\PsychShift\PsychShift\Assets\Editor\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB6CDCB-DF22-46F5-A5C6-ABC24DB0AFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B013E91-60E9-4F49-A072-CBD846851434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CBE73A3-79C0-44EA-87C7-E817604DF246}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Weapon</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Falloff Ratio</t>
+  </si>
+  <si>
+    <t>Bullets Per Shot</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -229,8 +235,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{814210BD-2EF3-4CD3-B1D8-4B2062515469}" name="Table3" displayName="Table3" ref="A1:I11" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:I11" xr:uid="{814210BD-2EF3-4CD3-B1D8-4B2062515469}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{814210BD-2EF3-4CD3-B1D8-4B2062515469}" name="Table3" displayName="Table3" ref="A1:J11" totalsRowShown="0" dataDxfId="10">
+  <autoFilter ref="A1:J11" xr:uid="{814210BD-2EF3-4CD3-B1D8-4B2062515469}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -240,17 +246,19 @@
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{62D694E6-FDBF-4FFC-A676-8631A653469F}" name="Weapon" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{BAEC8F8D-4E22-4E96-A936-46B900587AA0}" name="Damage" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{4067D311-D36E-4659-8730-204846B3B2D6}" name="Crit Dmg" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{49D0C156-22A0-4741-A51A-F896403C0F7A}" name="RoF" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{6C424D53-5C71-4E08-8C92-910CF38E342D}" name="Clip Size" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{FD941F29-CEDD-4CF5-BE20-409C308989E9}" name="Enemy Health" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{EB856784-23BE-4B72-B9B4-D337FA986716}" name="No Falloff range" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{3E4F649D-A500-44B5-8547-17EEB9FAF829}" name="Max Falloff Distance" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{C3FDC246-FDF0-4043-8FE6-AF2E781298B6}" name="Falloff Ratio" dataDxfId="0"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{62D694E6-FDBF-4FFC-A676-8631A653469F}" name="Weapon" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{BAEC8F8D-4E22-4E96-A936-46B900587AA0}" name="Damage" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4067D311-D36E-4659-8730-204846B3B2D6}" name="Crit Dmg" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{49D0C156-22A0-4741-A51A-F896403C0F7A}" name="RoF" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{6C424D53-5C71-4E08-8C92-910CF38E342D}" name="Clip Size" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FD941F29-CEDD-4CF5-BE20-409C308989E9}" name="Enemy Health" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{EB856784-23BE-4B72-B9B4-D337FA986716}" name="No Falloff range" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{3E4F649D-A500-44B5-8547-17EEB9FAF829}" name="Max Falloff Distance" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{C3FDC246-FDF0-4043-8FE6-AF2E781298B6}" name="Falloff Ratio" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{5E10BFF7-B155-49B1-842B-64127A777B80}" name="Bullets Per Shot" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -576,7 +584,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:J14"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +592,8 @@
     <col min="1" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="10" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="19" max="20" width="9.42578125" customWidth="1"/>
@@ -622,6 +631,9 @@
       <c r="I1" t="s">
         <v>27</v>
       </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -649,7 +661,10 @@
         <v>100</v>
       </c>
       <c r="I2" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -678,7 +693,10 @@
         <v>100</v>
       </c>
       <c r="I3" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -701,13 +719,16 @@
         <v>40</v>
       </c>
       <c r="G4" s="1">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -738,6 +759,9 @@
       <c r="I5" s="1">
         <v>0.5</v>
       </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -765,7 +789,10 @@
         <v>100</v>
       </c>
       <c r="I6" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -794,7 +821,10 @@
         <v>100</v>
       </c>
       <c r="I7" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -823,7 +853,10 @@
         <v>100</v>
       </c>
       <c r="I8" s="1">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -831,7 +864,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <v>1.5</v>
@@ -846,13 +879,16 @@
         <v>20</v>
       </c>
       <c r="G9" s="1">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -881,7 +917,10 @@
         <v>100</v>
       </c>
       <c r="I10" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -896,6 +935,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1019,11 +1059,11 @@
         <v>7</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" ref="B19:B27" si="0">ROUND((B2*(1/D2))*$C$17,0)</f>
+        <f>ROUND((B2*(1/D2))*J2*$C$17,0)</f>
         <v>250</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ref="C19:C27" si="1">B2*E2*$C$17</f>
+        <f t="shared" ref="C19:C27" si="0">B2*E2*$C$17</f>
         <v>2250</v>
       </c>
       <c r="D19" s="1" t="str">
@@ -1038,11 +1078,11 @@
         <v>7</v>
       </c>
       <c r="G19" s="1">
-        <f>ROUND(((B2*(1/D2))*$H$17)*C2*$H$16,0)</f>
+        <f>ROUND(((B2*(1/D2))*J2*$H$17)*C2*$H$16,0)</f>
         <v>750</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19:H27" si="2">B2*E2*$C$17</f>
+        <f t="shared" ref="H19:H27" si="1">B2*E2*$C$17</f>
         <v>2250</v>
       </c>
       <c r="I19" s="1" t="str">
@@ -1055,11 +1095,11 @@
         <v>8</v>
       </c>
       <c r="B20" s="1">
+        <f t="shared" ref="B20:B27" si="2">ROUND((B3*(1/D3))*J3*$C$17,0)</f>
+        <v>117</v>
+      </c>
+      <c r="C20" s="1">
         <f t="shared" si="0"/>
-        <v>117</v>
-      </c>
-      <c r="C20" s="1">
-        <f t="shared" si="1"/>
         <v>700</v>
       </c>
       <c r="D20" s="1" t="str">
@@ -1074,16 +1114,16 @@
         <v>8</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" ref="G20:G27" si="4">ROUND((B3*(1/D3))*$H$17+((B3*(1/D3))*$H$17)*C3*$H$16,0)</f>
-        <v>350</v>
+        <f t="shared" ref="G20:G27" si="4">ROUND(((B3*(1/D3))*J3*$H$17)*C3*$H$16,0)</f>
+        <v>233</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>700</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" ref="I20:I27" si="5">CONCATENATE(ROUND(VLOOKUP($I$18, A:F, 6, FALSE)/G20,3)," Sec")</f>
-        <v>0.286 Sec</v>
+        <v>0.429 Sec</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1091,7 +1131,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="C21" s="1">
@@ -1111,15 +1151,15 @@
       </c>
       <c r="G21" s="1">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.1 Sec</v>
+        <v>0.167 Sec</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1127,11 +1167,11 @@
         <v>10</v>
       </c>
       <c r="B22" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C22" s="1">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="C22" s="1">
-        <f t="shared" si="1"/>
         <v>600</v>
       </c>
       <c r="D22" s="1" t="str">
@@ -1147,15 +1187,15 @@
       </c>
       <c r="G22" s="1">
         <f t="shared" si="4"/>
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.4 Sec</v>
+        <v>0.667 Sec</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1163,11 +1203,11 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="C23" s="1">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="C23" s="1">
-        <f t="shared" si="1"/>
         <v>1600</v>
       </c>
       <c r="D23" s="1" t="str">
@@ -1183,15 +1223,15 @@
       </c>
       <c r="G23" s="1">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1600</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1 Sec</v>
+        <v>1.667 Sec</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1199,11 +1239,11 @@
         <v>12</v>
       </c>
       <c r="B24" s="1">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="C24" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C24" s="1">
-        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="D24" s="1" t="str">
@@ -1219,15 +1259,15 @@
       </c>
       <c r="G24" s="1">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>2.632 Sec</v>
+        <v>4.348 Sec</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1235,11 +1275,11 @@
         <v>11</v>
       </c>
       <c r="B25" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="C25" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="D25" s="1" t="str">
@@ -1255,15 +1295,15 @@
       </c>
       <c r="G25" s="1">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>2 Sec</v>
+        <v>3.333 Sec</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1271,35 +1311,35 @@
         <v>14</v>
       </c>
       <c r="B26" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="C26" s="1">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="C26" s="1">
-        <f t="shared" si="1"/>
-        <v>1200</v>
+        <v>90</v>
       </c>
       <c r="D26" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>2.5 Sec</v>
+        <v>3.333 Sec</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="3"/>
-        <v>2.5 Sec</v>
+        <v>3.333 Sec</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="2"/>
-        <v>1200</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1 Sec</v>
+        <v>2.222 Sec</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1307,11 +1347,11 @@
         <v>15</v>
       </c>
       <c r="B27" s="1">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="C27" s="1">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="C27" s="1">
-        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="D27" s="1" t="str">
@@ -1327,15 +1367,15 @@
       </c>
       <c r="G27" s="1">
         <f t="shared" si="4"/>
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.2 Sec</v>
+        <v>0.333 Sec</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
csv.. update it... please
</commit_message>
<xml_diff>
--- a/PsychShift/Assets/Editor/CSV/EnemyExcelChart.xlsx
+++ b/PsychShift/Assets/Editor/CSV/EnemyExcelChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxth\OneDrive\Desktop\PsychShift\PsychShift\Assets\Editor\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82306BF5-A617-4A3F-ABAD-6B6DB751C51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7563E5B9-AD78-4903-BDBB-334A50F8FFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CBE73A3-79C0-44EA-87C7-E817604DF246}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
         <v>50</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="D2" s="1">
         <v>0.2</v>
@@ -675,7 +675,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D3" s="1">
         <v>0.3</v>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="G19" s="1">
         <f>ROUND(((B2*(1/D2))*J2*$H$17)*C2*$H$16,0)</f>
-        <v>750</v>
+        <v>375</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" ref="H19:H27" si="1">B2*E2*$C$17</f>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="I19" s="1" t="str">
         <f>CONCATENATE(ROUND(VLOOKUP($I$18, A:F, 6, FALSE)/G19,3)," Sec")</f>
-        <v>0.133 Sec</v>
+        <v>0.267 Sec</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" ref="G20:G27" si="4">ROUND(((B3*(1/D3))*J3*$H$17)*C3*$H$16,0)</f>
-        <v>233</v>
+        <v>175</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" ref="I20:I27" si="5">CONCATENATE(ROUND(VLOOKUP($I$18, A:F, 6, FALSE)/G20,3)," Sec")</f>
-        <v>0.429 Sec</v>
+        <v>0.571 Sec</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>